<commit_message>
Lots of UI + restart/backtomap funtionality
</commit_message>
<xml_diff>
--- a/Maps/Maps/WoodedPath.xlsx
+++ b/Maps/Maps/WoodedPath.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spec\Documents\GitHub\TowerDefense\Maps\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92174572-3CE4-41D5-BE66-4F8EAFC753BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505706A2-A610-4EE4-9F9D-EA01DC0C6627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9810" windowWidth="29040" windowHeight="15840" xr2:uid="{7C7806C9-AC08-4287-BFE3-355EE0D4C54D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7C7806C9-AC08-4287-BFE3-355EE0D4C54D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1181,7 +1181,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <selection pane="topRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>